<commit_message>
minor fixes to examples, profiles
</commit_message>
<xml_diff>
--- a/prototype/alr_ig/output/StructureDefinition-ext-serviceCount.xlsx
+++ b/prototype/alr_ig/output/StructureDefinition-ext-serviceCount.xlsx
@@ -206,7 +206,7 @@
     <t>Element.extension</t>
   </si>
   <si>
-    <t>category</t>
+    <t>serviceCountCode</t>
   </si>
   <si>
     <t>An Extension</t>
@@ -437,7 +437,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="28.2734375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="12.6640625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="17.24609375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="12.3828125" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>

</xml_diff>